<commit_message>
feat: Enhance labour tracking with new labour role functionality   - Added `labour_role` column to `daily_attendance` table for accurate BOQ cost tracking. - Implemented logic in `boq_tracking_controller.py` to determine labour roles based on attendance records, assignments, and worker skills. - Updated `clock_in_worker` function in `labour_controller.py` to accept and store labour roles during clock-in. - Created migrations to backfill existing attendance records with appropriate labour roles and fix records with "Multiple Skills". - Enhanced frontend components to support labour role selection during clock-in and display roles in attendance logs.  This update improves the accuracy of labour cost tracking and enhances the user experience by linking attendance to specific labour roles.
</commit_message>
<xml_diff>
--- a/MSQ App Version History.xlsx
+++ b/MSQ App Version History.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="v1.0.1.5 Changelog" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="v1.0.1.4 changelog" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="v1.0.1.3 Changelog" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="v1.0.1.2 Changelog" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Version History Summary" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Deployment Notes" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="v1.0.2.1 Changelog" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="v1.0.1.5 Changelog" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="v1.0.1.4 changelog" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="v1.0.1.3 Changelog" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="v1.0.1.2 Changelog" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Version History Summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Deployment Notes" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -21,7 +22,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <name val="Calibri"/>
@@ -114,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -167,6 +170,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +541,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -583,106 +590,104 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1.0.2.1</t>
+        </is>
+      </c>
+      <c r="B2" s="22" t="n">
+        <v>46040</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Released</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>DevOps Team</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Latest - 68 features/fixes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>1.0.1.5</t>
         </is>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B3" s="5" t="n">
         <v>46022</v>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>Released</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>DevOps Team</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>Latest - 22 features/fixes</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>Previous - 22 features/fixes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>1.0.1.4</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B4" s="2" t="n">
         <v>46011</v>
       </c>
-      <c r="C3" s="1" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>Released</t>
         </is>
       </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>DevOps Team</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>Latest - 20 features/fixes</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>1.0.1.3</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>2025-12-16</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>Released</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>Production</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>DevOps Team</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>Latest - 15 features/fixes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>1.0.1.2</t>
+          <t>1.0.1.3</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -702,19 +707,19 @@
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>Stable - 35 features/fixes</t>
+          <t>Latest - 15 features/fixes</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>1.0.1.1</t>
+          <t>1.0.1.2</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -734,37 +739,69 @@
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>Previous - 15 bug fixes</t>
+          <t>Stable - 35 features/fixes</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
+          <t>1.0.1.1</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-12</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Released</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>Production</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>DevOps Team</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Previous - 15 bug fixes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
           <t>1.0.1.0</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>2025-10-01</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>Archived</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>Production</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
         <is>
           <t>DevOps Team</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F8" s="3" t="inlineStr">
         <is>
           <t>Legacy version</t>
         </is>
@@ -776,6 +813,2442 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Item#</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Release Date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Severity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Profit Comparison</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Added Profit Comparison PDF export functionality</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Labour Workflow</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Enhanced labour workflow tracking with planned vs actual hours and costs calculation</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>BOQ Tracking</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Fetch actual labour data from DailyAttendance instead of LabourTracking for accurate reporting</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Labour Workflow</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Added comprehensive labour workflow tracking with requisition and payment lock details</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Labour UI</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Enhanced labour section visual design with clear differentiation and professional styling</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2026-01-15</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Profit Comparison</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Added labour tracking details to Profit Comparison page</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>MEP Dashboard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Implemented MEP Dashboard with role-based viewing and admin MEP role support</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Attendance</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Added quick select dropdown for auto-selecting workers by low-rate, high-rate, single-skill, or multi-skill criteria</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Attendance</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Enhanced attendance management with requisition linking, bulk actions, and date grouping in AttendanceLock</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Arrival Confirmation</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Added functionality to handle late arrivals with bulk confirmation logic and no_show status</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Change Request</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Added routed_to_store status for material routing through Production Manager workflow</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>User Projects API</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Implemented user projects retrieval API based on user roles for AttendanceLock</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SE Movement History</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Added SE movement history endpoint for ADN/ARDN tracking in assigned projects</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Asset Requisition</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Added asset requisition notifications (created, approved, rejected, dispatched) with email support</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Asset Requisition</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Added AssetRequisitionApprovals component for project managers</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Asset Dispatch</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Updated asset dispatch to support linked requisitions with pre-filled delivery notes</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Asset Receipt</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Enhanced asset requisition receipt confirmation with user email tracking and ADN status updates</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Stock Out</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Implemented lazy loading for material requests with categorized states (pending, approved, completed, rejected)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Asset Disposal</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Implemented pending disposal request handling with deferred asset reduction until approval</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Asset Disposal</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Added tabbed filtering for disposal items (pending/approved) in AssetDisposalPage</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Site Assets</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Added quantity management for returned items with validation</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Inventory</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Enhanced inventory processing with mandatory notes for disposal actions</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Payroll</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Enhanced payroll summary and attendance management with requisition details integration</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Inventory PDF</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Added inventory PDF generation functionality</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Split API</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Implemented Split API code changes across frontend and backend</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>BOQ Tracking</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Enhanced BOQ tracking logic to fetch requisitions from both deprecated and JSONB columns</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Labour Workflow</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Added professional clean labour workflow with work history tracking</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>MEP/PM Roles</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Enhanced MEP and PM role functionalities with improved filtering and pagination support</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>PM Dashboard</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Updated PM and Admin PM dashboard code changes</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>UI Components</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Enhanced UI with collapsible requisition groups and selection indicators</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Email Service</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Updated email service to embed logo images for better compatibility</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Frontend Performance</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Improved frontend components with memoization techniques for better performance</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Labour Management</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Added labour edit, send to PM, pagination, and tab count features in PM/SS roles</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Labour View</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Role-based labour display and multiple labour view in SS, PM, PRM roles</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Multi Labour Split</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Multi labour split views across PM, PRM, SS roles</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Asset Requisition</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Added project ID validation and selection for asset requisitions</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Site Assets UI</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Enhanced SiteAssets UI consistency with simplified color palette and accessibility improvements</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Asset Routes</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Refactored asset delivery note and stock in routes with blueprint structure</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Asset PDF</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Improved asset PDF layout by removing Notes column and adjusting widths</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Asset Navigation</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Updated asset navigation paths in production manager components</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Material Receipts</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Optimistic updates and syncing states in material receipts for better UX</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Confirmation Modal</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Enhanced accessibility with aria-describedby attribute</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Production/TD Role</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Added Area and notes setting in production and TD roles</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>SS Role</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Material create to list a project in SS role</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2026-01-17</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>BOQ/Labour</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Critical performance and security improvements for labour workflow</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2026-01-15</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Profit Comparison</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Added Technical Director access to Profit Comparison page</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>TD Role</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Fixed TD role purchase section pending tab table</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Attendance</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Fixed number of workers present calculation</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2026-01-13</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Auto Select</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Bug fix for auto select functionality</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>SE Asset Request</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Quantity fix in the SE asset request</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>EST/PM Roles</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>EST rejected count fix and multi PM assign SS fix</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>SS Return API</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>SS return API fixes in SS role</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>BOQ Count</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>BOQ count fix in TD role</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Asset Deduction</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Asset double deduction fix in inventory</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Input Area</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Input area fixes across multiple components</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Asset Edit</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Asset edit and popup view fixes</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>PM Role Assets</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Role-based asset display for PM role</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>PM Labour Lock</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Role-based labour lock display in PM role</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Disposal Rejection</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Fixed rejection handling in disposal approvals with proper user feedback</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Return Material</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Return material raised to process completed code fix</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Completed Tab</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Completed tab BOQ view details issue fix in PM</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Request Complete</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Request complete SS code fix</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2026-01-14</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Codebase</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Removed backup files and unused components for cleaner codebase</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2026-01-12</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>MEP Role</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Removed debug print statement in MEP role</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Test Files</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Removed test file from codebase</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Reports</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Removed obsolete M2StoreReports component</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Backend</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Removed unused code in backend</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Codebase</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Maintenance</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Removed multiple obsolete files including PDFs, scripts, and markdown documents</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2257,7 +4730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3045,7 +5518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3634,7 +6107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4958,13 +7431,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G3:G5"/>
@@ -5020,27 +7493,27 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>1.0.1.5</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>46022</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>14</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1.0.2.1</t>
+        </is>
+      </c>
+      <c r="B2" s="22" t="n">
+        <v>46040</v>
+      </c>
+      <c r="C2" t="n">
+        <v>68</v>
+      </c>
+      <c r="D2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -5049,52 +7522,50 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>1.0.1.4</t>
+          <t>1.0.1.5</t>
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>46011</v>
+        <v>46022</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>14</v>
       </c>
       <c r="F3" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
+        <is>
+          <t>Stable</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>1.0.1.4</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>46011</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>5</v>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>Stable</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>1.0.1.3</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>2025-12-16</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>3</v>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
@@ -5105,25 +7576,25 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>1.0.1.2</t>
+          <t>1.0.1.3</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
@@ -5134,56 +7605,85 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>1.0.1.1</t>
+          <t>1.0.1.2</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>Legacy</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>1.0.1.0</t>
+          <t>1.0.1.1</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-12</t>
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Legacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>1.0.1.0</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
         <is>
           <t>Archived</t>
         </is>
@@ -5194,7 +7694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5233,7 +7733,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>MSQ</t>
+          <t>1.0.2.1</t>
         </is>
       </c>
     </row>
@@ -5245,7 +7745,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>1.0.1.4</t>
+          <t>1.0.2.0</t>
         </is>
       </c>
     </row>
@@ -5255,10 +7755,8 @@
           <t>Previous Version</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>1.0.1.3</t>
-        </is>
+      <c r="B4" s="23" t="n">
+        <v>46040</v>
       </c>
     </row>
     <row r="5">
@@ -5267,8 +7765,10 @@
           <t>Last Updated</t>
         </is>
       </c>
-      <c r="B5" s="7" t="n">
-        <v>46011</v>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>DevOps Team</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -5291,7 +7791,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Production</t>
+          <t>1 (Labour workflow performance)</t>
         </is>
       </c>
     </row>
@@ -5303,7 +7803,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>3 (Notification, LPO, Vendor Approval)</t>
+          <t>Profit Comparison PDF, Labour Workflow, MEP Dashboard, Asset Requisition, Split API</t>
         </is>
       </c>
     </row>
@@ -5315,7 +7815,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Inventroy</t>
+          <t>2026-01-25</t>
         </is>
       </c>
     </row>

</xml_diff>